<commit_message>
dokoncena S-48-50/100 pridany nove obrazky k D-48-50 pokracovani popisu pinu D-48-50
</commit_message>
<xml_diff>
--- a/docs/Manual/source/CZ/tab/connectors.xlsx
+++ b/docs/Manual/source/CZ/tab/connectors.xlsx
@@ -5,19 +5,24 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="X1_24V_5pin_BCZ" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="X2_48_DC_1778065" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="X8_IO_22pin_BCZ" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="X10_CAN_4pin_BCZ" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="LEDsigAx12" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="X5_FBE_12pin_BCZ" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="X6_FB1_8pin_BCZ" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="X7_FB2_8pin_BCZ" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="X3_M1_6pin_BLZP" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="X4_M2_6pin_BLZP" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="rozcestnik" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="X1_24V_5pin_BCZ" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="X2_48_DC_1778065" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="X8_IO_22pin_BCZ" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="X10_CAN_4pin_BCZ" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="LEDsigAx12" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="X5_FBE_12pin_BCZ" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="X6_FB1_8pin_BCZ" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="X7_FB2_8pin_BCZ" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="X3_M1_6pin_BLZP" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="X4_M2_6pin_BLZP" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="X1_24V_5pin_Microlock" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="X3_DCbus_2pin_pressfit" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="X3_M1_3pin_pressfit" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="X4_BR_4pin_Microlock" sheetId="15" state="visible" r:id="rId16"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -29,7 +34,91 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="153">
+  <si>
+    <t xml:space="preserve">Toto je sešit se zdrojovými tabulkami popisu konektorů TGZ/TGS v češtině. Každý list odpovídá jednomu unikátnímu typu konektoru. Jelikož se často konektory v rámci TGZ opakují (typicky ty na řídicií desce), jsou zde jen jednou. Tj. Např. IO konektor 22pin weidmuller BCZ se používá pořád dokola, je zde tedy zanesen jen jednou jako „X8_IO_22pin_BCZ“</t>
+  </si>
+  <si>
+    <t xml:space="preserve">výrobce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">řada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">počet OS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">napětí</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jmen. Proud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">špičkový proud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">typ konektoru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#X1_24V_5pin_Microlock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#X8_IO_22pin_BCZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#X10_CAN_4pin_BCZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FB1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#X6_FB1_8pin_BCZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FB2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#X7_FB2_8pin_BCZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FBE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#X5_FBE_12pin_BCZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#X3_M1_3pin_pressfit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dcbus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#X3_DCbus_2pin_pressfit</t>
+  </si>
   <si>
     <t xml:space="preserve">Pin č.</t>
   </si>
@@ -399,6 +488,48 @@
   <si>
     <t xml:space="preserve">Fáze U</t>
   </si>
+  <si>
+    <t xml:space="preserve">0,13 ~ 0,32 mm2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Připojení</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oko M5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+6 ~ +50 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fáze W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fáze V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fáze U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-BR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+BR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-TERM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Tepl. čidla mot.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+TERM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ Tepl. čidla mot.</t>
+  </si>
 </sst>
 </file>
 
@@ -407,7 +538,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -433,6 +564,13 @@
       <charset val="238"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
       <vertAlign val="superscript"/>
       <sz val="10"/>
       <name val="Arial"/>
@@ -446,12 +584,18 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF5CE"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -488,12 +632,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -506,6 +666,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFF5CE"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -514,104 +734,257 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.23828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="18.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="31.81"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="B8" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="C8" s="0" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="D8" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="E8" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="F8" s="0" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="G8" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="H8" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="B9" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="0" t="s">
+      <c r="C9" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D9" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G9" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="0" t="s">
+      <c r="H9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="0" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>6</v>
+      <c r="H10" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D12" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D13" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D14" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D15" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D16" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D17" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>250</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:H6"/>
+    <mergeCell ref="E9:E16"/>
+    <mergeCell ref="F9:F16"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="H9" location="X1_24V_5pin_Microlock!A1" display="#X1_24V_5pin_Microlock"/>
+    <hyperlink ref="H10" location="X8_IO_22pin_BCZ!A1" display="#X8_IO_22pin_BCZ"/>
+    <hyperlink ref="H11" location="X10_CAN_4pin_BCZ!A1" display="#X10_CAN_4pin_BCZ"/>
+    <hyperlink ref="H12" location="X6_FB1_8pin_BCZ!A1" display="#X6_FB1_8pin_BCZ"/>
+    <hyperlink ref="H13" location="X7_FB2_8pin_BCZ!A1" display="#X7_FB2_8pin_BCZ"/>
+    <hyperlink ref="H14" location="X5_FBE_12pin_BCZ!A1" display="#X5_FBE_12pin_BCZ"/>
+    <hyperlink ref="H15" location="X3_M1_3pin_pressfit!A1" display="#X3_M1_3pin_pressfit"/>
+    <hyperlink ref="H16" location="X3_DCbus_2pin_pressfit!A1" display="#X3_DCbus_2pin_pressfit"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -629,11 +1002,11 @@
   </sheetPr>
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
@@ -642,16 +1015,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -659,13 +1032,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>99</v>
+        <v>127</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>100</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -673,13 +1046,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>100</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -687,13 +1060,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>103</v>
+        <v>131</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>100</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -701,13 +1074,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>100</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -715,13 +1088,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>107</v>
+        <v>135</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>108</v>
+        <v>136</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>100</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -729,22 +1102,526 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>109</v>
+        <v>137</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>100</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="1"/>
+      <c r="C18" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.72"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="5"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="18.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.72"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="5"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.72"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="5"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="18.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
@@ -757,26 +1634,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="18.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.83"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -784,13 +1666,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -798,13 +1680,55 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>17</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -823,30 +1747,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.72"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -854,13 +1774,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -868,293 +1788,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="B16" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1173,30 +1813,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1204,13 +1844,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1218,13 +1858,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1232,13 +1872,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1246,13 +1886,265 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C12" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D12" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
         <v>22</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1271,39 +2163,86 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>70</v>
+        <v>29</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>71</v>
+      <c r="A2" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>72</v>
+        <v>89</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>73</v>
+      <c r="A3" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>74</v>
+        <v>91</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1322,203 +2261,40 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.62"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
+      <c r="A2" s="0" t="s">
+        <v>99</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>13</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
+      <c r="A3" s="0" t="s">
+        <v>101</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="1"/>
+        <v>102</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1539,10 +2315,10 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
@@ -1551,16 +2327,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1568,13 +2344,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1582,13 +2358,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>81</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1596,13 +2372,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1610,13 +2386,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1624,13 +2400,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>81</v>
+        <v>113</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1638,13 +2414,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1652,13 +2428,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>13</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1666,17 +2442,73 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>96</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="1"/>
+      <c r="C18" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1700,7 +2532,7 @@
       <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
@@ -1709,16 +2541,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1726,13 +2558,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1740,13 +2572,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1754,13 +2586,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>87</v>
+        <v>115</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1768,13 +2600,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1782,13 +2614,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1796,13 +2628,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>94</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1810,13 +2642,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1824,17 +2656,17 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="1"/>
+      <c r="C18" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1855,10 +2687,10 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
@@ -1867,16 +2699,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>2</v>
+        <v>104</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>3</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1884,13 +2716,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1898,13 +2730,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1912,13 +2744,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1926,13 +2758,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1940,13 +2772,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1954,17 +2786,45 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>110</v>
-      </c>
       <c r="D7" s="0" t="s">
-        <v>100</v>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="1"/>
+      <c r="C18" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
pridan TGZ-S-48-100/250 (chybi jeste rozmery a mounting)
</commit_message>
<xml_diff>
--- a/docs/Manual/source/CZ/tab/connectors.xlsx
+++ b/docs/Manual/source/CZ/tab/connectors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="rozcestnik" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,6 +23,14 @@
     <sheet name="X3_DCbus_2pin_pressfit" sheetId="13" state="visible" r:id="rId14"/>
     <sheet name="X3_M1_3pin_pressfit" sheetId="14" state="visible" r:id="rId15"/>
     <sheet name="X4_BR_4pin_Microlock" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="X2_DCbus_3pin_wago_2636" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="X3_M1_4pin_wago_2626" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="X4_M2_4pin_wago_2626" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="XBR_BR_6pin_BLF" sheetId="19" state="visible" r:id="rId20"/>
+    <sheet name="X1_24V_5pin_Microfit" sheetId="20" state="visible" r:id="rId21"/>
+    <sheet name="P7_BR_4pin_Microfit" sheetId="21" state="visible" r:id="rId22"/>
+    <sheet name="P8_BR_4pin_Microfit" sheetId="22" state="visible" r:id="rId23"/>
+    <sheet name="P3_Term_2pin_Microfit" sheetId="23" state="visible" r:id="rId24"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -34,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="179">
   <si>
     <t xml:space="preserve">Toto je sešit se zdrojovými tabulkami popisu konektorů TGZ/TGS v češtině. Každý list odpovídá jednomu unikátnímu typu konektoru. Jelikož se často konektory v rámci TGZ opakují (typicky ty na řídicií desce), jsou zde jen jednou. Tj. Např. IO konektor 22pin weidmuller BCZ se používá pořád dokola, je zde tedy zanesen jen jednou jako „X8_IO_22pin_BCZ“</t>
   </si>
@@ -530,13 +538,92 @@
   <si>
     <t xml:space="preserve">+ Tepl. čidla mot.</t>
   </si>
+  <si>
+    <t xml:space="preserve">uzemnění</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,75 ~ 16 mm2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,2 ~ 10 mm2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-B2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Brzda motor 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,13 ~ 2,5 mm2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ Brzda motor 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">– Napájení brzdy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ Napájení brzdy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-B1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Brzda motor 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+B1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ Brzda motor 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+24V DC napájení řízení</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,05 ~ 0,75 mm2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VCC_OUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Výstup +24 VDC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+24V DC napájení brzdy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VCCD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+24V DC napájení diag. brzdy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ Brzda servomotoru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Brzda servomotoru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nezapojuje se</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0V napájení řízení</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TERM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teplotní čidlo PT1000</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -632,7 +719,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -655,6 +742,10 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -736,8 +827,8 @@
   </sheetPr>
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.23828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1450,7 +1541,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1538,7 +1629,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1622,6 +1713,429 @@
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.72"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="5"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.72"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="5"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.72"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="5"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.72"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="str">
+        <f aca="false">+B2</f>
+        <v>-B2</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="5"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
@@ -1729,6 +2243,392 @@
       </c>
       <c r="D6" s="0" t="s">
         <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed /site folder added S-48-100/250/300/425 added S-230 added D-320 (TBD)
</commit_message>
<xml_diff>
--- a/docs/Manual/source/CZ/tab/connectors.xlsx
+++ b/docs/Manual/source/CZ/tab/connectors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="22"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="rozcestnik" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,6 +31,9 @@
     <sheet name="P7_BR_4pin_Microfit" sheetId="21" state="visible" r:id="rId22"/>
     <sheet name="P8_BR_4pin_Microfit" sheetId="22" state="visible" r:id="rId23"/>
     <sheet name="P3_Term_2pin_Microfit" sheetId="23" state="visible" r:id="rId24"/>
+    <sheet name="X4_M1_6pin_SLS" sheetId="24" state="visible" r:id="rId25"/>
+    <sheet name="X2_PWR_10pin_BLZP" sheetId="25" state="visible" r:id="rId26"/>
+    <sheet name="X2_320_DC_1778078" sheetId="26" state="visible" r:id="rId27"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -42,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="199">
   <si>
     <t xml:space="preserve">Toto je sešit se zdrojovými tabulkami popisu konektorů TGZ/TGS v češtině. Každý list odpovídá jednomu unikátnímu typu konektoru. Jelikož se často konektory v rámci TGZ opakují (typicky ty na řídicií desce), jsou zde jen jednou. Tj. Např. IO konektor 22pin weidmuller BCZ se používá pořád dokola, je zde tedy zanesen jen jednou jako „X8_IO_22pin_BCZ“</t>
   </si>
@@ -615,6 +618,66 @@
   </si>
   <si>
     <t xml:space="preserve">Teplotní čidlo PT1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,2 ~ 2,5 mm2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Střední pracovní vodič</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fáze </t>
+  </si>
+  <si>
+    <t xml:space="preserve">+RB </t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ Brzdný odpor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-RB </t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Brzdný odpor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+DC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ Napájení meziobvodu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-DC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Napájení meziobvodu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">T+ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ Termistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T- </t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Termistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+140 ~ +320V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max. 6 mm2</t>
   </si>
 </sst>
 </file>
@@ -724,16 +787,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -746,6 +805,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -831,9 +894,9 @@
       <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.23828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.25390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="31.81"/>
   </cols>
@@ -980,7 +1043,7 @@
       <c r="G11" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -993,7 +1056,7 @@
       <c r="G12" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1006,7 +1069,7 @@
       <c r="G13" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1019,7 +1082,7 @@
       <c r="G14" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1032,7 +1095,7 @@
       <c r="G15" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1045,7 +1108,7 @@
       <c r="G16" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1097,7 +1160,7 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
@@ -1203,7 +1266,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="5"/>
+      <c r="C18" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1227,7 +1290,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
@@ -1333,7 +1396,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="5"/>
+      <c r="C18" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1357,7 +1420,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="18.38"/>
@@ -1470,7 +1533,7 @@
       <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
@@ -1520,7 +1583,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="5"/>
+      <c r="C18" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1544,7 +1607,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
@@ -1608,7 +1671,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="5"/>
+      <c r="C18" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1632,7 +1695,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="18.38"/>
@@ -1731,7 +1794,7 @@
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
@@ -1795,7 +1858,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="5"/>
+      <c r="C18" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1819,7 +1882,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
@@ -1897,7 +1960,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="5"/>
+      <c r="C18" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1921,7 +1984,7 @@
       <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
@@ -1999,7 +2062,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="5"/>
+      <c r="C18" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2023,7 +2086,7 @@
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.23"/>
@@ -2048,7 +2111,7 @@
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>156</v>
       </c>
       <c r="C2" s="0" t="s">
@@ -2105,7 +2168,7 @@
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>162</v>
       </c>
       <c r="C6" s="0" t="s">
@@ -2119,7 +2182,7 @@
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>164</v>
       </c>
       <c r="C7" s="0" t="s">
@@ -2130,7 +2193,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="5"/>
+      <c r="C18" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2154,7 +2217,7 @@
       <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="18.38"/>
@@ -2267,11 +2330,11 @@
       <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.83"/>
   </cols>
   <sheetData>
@@ -2381,7 +2444,7 @@
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.38"/>
@@ -2481,7 +2544,7 @@
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.38"/>
@@ -2577,11 +2640,11 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H44" activeCellId="0" sqref="H44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.38"/>
@@ -2629,6 +2692,405 @@
       </c>
       <c r="D3" s="0" t="s">
         <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.72"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="4"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.72"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="4"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -2653,7 +3115,7 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -2719,7 +3181,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.72"/>
@@ -3069,7 +3531,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.33"/>
@@ -3167,7 +3629,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.62"/>
   </cols>
@@ -3218,7 +3680,7 @@
       <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
@@ -3408,7 +3870,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="5"/>
+      <c r="C18" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3432,7 +3894,7 @@
       <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
@@ -3566,7 +4028,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="5"/>
+      <c r="C18" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3590,7 +4052,7 @@
       <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
@@ -3724,7 +4186,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="5"/>
+      <c r="C18" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
pridany vsechny S-400 zaciname D-560
</commit_message>
<xml_diff>
--- a/docs/Manual/source/CZ/tab/connectors.xlsx
+++ b/docs/Manual/source/CZ/tab/connectors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="25"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="27"/>
   </bookViews>
   <sheets>
     <sheet name="rozcestnik" sheetId="1" state="visible" r:id="rId2"/>
@@ -34,6 +34,8 @@
     <sheet name="X4_M1_6pin_SLS" sheetId="24" state="visible" r:id="rId25"/>
     <sheet name="X2_PWR_10pin_BLZP" sheetId="25" state="visible" r:id="rId26"/>
     <sheet name="X2_320_DC_1778078" sheetId="26" state="visible" r:id="rId27"/>
+    <sheet name="X4_M1_6pin_BLF" sheetId="27" state="visible" r:id="rId28"/>
+    <sheet name="X2_PWR_12pin_BLZ" sheetId="28" state="visible" r:id="rId29"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="214">
   <si>
     <t xml:space="preserve">Toto je sešit se zdrojovými tabulkami popisu konektorů TGZ/TGS v češtině. Každý list odpovídá jednomu unikátnímu typu konektoru. Jelikož se často konektory v rámci TGZ opakují (typicky ty na řídicií desce), jsou zde jen jednou. Tj. Např. IO konektor 22pin weidmuller BCZ se používá pořád dokola, je zde tedy zanesen jen jednou jako „X8_IO_22pin_BCZ“</t>
   </si>
@@ -678,6 +680,51 @@
   </si>
   <si>
     <t xml:space="preserve">Max. 6 mm2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,5 ~ 2,5 mm2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fáze 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fáze 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fáze 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RBin </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brzdný odpor interní</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volba brzdného odporu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RBex </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brzdný odpor externí</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+Termistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-Termistor</t>
   </si>
 </sst>
 </file>
@@ -894,9 +941,9 @@
       <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.25390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="31.81"/>
   </cols>
@@ -1160,7 +1207,7 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
@@ -1290,7 +1337,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
@@ -1420,7 +1467,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="18.38"/>
@@ -1533,7 +1580,7 @@
       <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
@@ -1607,7 +1654,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
@@ -1695,7 +1742,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="18.38"/>
@@ -1794,7 +1841,7 @@
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
@@ -1882,7 +1929,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
@@ -1984,7 +2031,7 @@
       <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
@@ -2083,10 +2130,10 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="F40" activeCellId="0" sqref="F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.23"/>
@@ -2217,7 +2264,7 @@
       <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="18.38"/>
@@ -2330,7 +2377,7 @@
       <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.38"/>
@@ -2444,7 +2491,7 @@
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.38"/>
@@ -2544,7 +2591,7 @@
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.38"/>
@@ -2644,7 +2691,7 @@
       <selection pane="topLeft" activeCell="H44" activeCellId="0" sqref="H44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.38"/>
@@ -2716,7 +2763,7 @@
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
@@ -2843,10 +2890,10 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+      <selection pane="topLeft" activeCell="E42" activeCellId="0" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.79"/>
@@ -3028,11 +3075,11 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.1"/>
   </cols>
@@ -3091,6 +3138,347 @@
       </c>
       <c r="D4" s="0" t="s">
         <v>198</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.72"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="4"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.72"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -3115,7 +3503,7 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -3181,7 +3569,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.72"/>
@@ -3531,7 +3919,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.33"/>
@@ -3629,7 +4017,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.62"/>
   </cols>
@@ -3680,7 +4068,7 @@
       <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
@@ -3894,7 +4282,7 @@
       <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>
@@ -4052,7 +4440,7 @@
       <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.78"/>

</xml_diff>

<commit_message>
Pridana kategorie napajece TGS Pridan TGS-320 a cca dokoncen Pridan TGS-560-50_100 (jen slozka) Uprava vsech popisu konektoru na bile s cernym lemem + vsechny jsou SVG
</commit_message>
<xml_diff>
--- a/docs/Manual/source/CZ/tab/connectors.xlsx
+++ b/docs/Manual/source/CZ/tab/connectors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="29"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="35"/>
   </bookViews>
   <sheets>
     <sheet name="rozcestnik" sheetId="1" state="visible" r:id="rId3"/>
@@ -38,6 +38,12 @@
     <sheet name="X2_PWR_12pin_BLZ" sheetId="28" state="visible" r:id="rId30"/>
     <sheet name="X2_D560DCbus" sheetId="29" state="visible" r:id="rId31"/>
     <sheet name="X3_M1_4pin_wago_2636" sheetId="30" state="visible" r:id="rId32"/>
+    <sheet name="X4_M2_4pin_wago_2636" sheetId="31" state="visible" r:id="rId33"/>
+    <sheet name="X14_BR1_4pin_LSF" sheetId="32" state="visible" r:id="rId34"/>
+    <sheet name="X15_BR2_4pin_LSF" sheetId="33" state="visible" r:id="rId35"/>
+    <sheet name="X1_ACIN_PC5" sheetId="34" state="visible" r:id="rId36"/>
+    <sheet name="X2_DC_8pin_PC5" sheetId="35" state="visible" r:id="rId37"/>
+    <sheet name="X3_DO_4pin_BCZ" sheetId="36" state="visible" r:id="rId38"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -49,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="243">
   <si>
     <t xml:space="preserve">Toto je sešit se zdrojovými tabulkami popisu konektorů TGZ/TGS v češtině. Každý list odpovídá jednomu unikátnímu typu konektoru. Jelikož se často konektory v rámci TGZ opakují (typicky ty na řídicií desce), jsou zde jen jednou. Tj. Např. IO konektor 22pin weidmuller BCZ se používá pořád dokola, je zde tedy zanesen jen jednou jako „X8_IO_22pin_BCZ“</t>
   </si>
@@ -723,9 +729,15 @@
     <t xml:space="preserve">Brzdný odpor externí</t>
   </si>
   <si>
+    <t xml:space="preserve">T+</t>
+  </si>
+  <si>
     <t xml:space="preserve">+Termistor</t>
   </si>
   <si>
+    <t xml:space="preserve">T-</t>
+  </si>
+  <si>
     <t xml:space="preserve">-Termistor</t>
   </si>
   <si>
@@ -742,6 +754,72 @@
   </si>
   <si>
     <t xml:space="preserve">- DC bus vstup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Brzda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,13 ~ 1,5 mm2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ Brzda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fáze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  + DC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - DC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  PE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  SEL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  + RB </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - RB </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  + T </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - T </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RDY1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signál „Ready“ kontakt 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RDY2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signál „Ready“ kontakt 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERR1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signál „Error“ kontakt 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERR2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signál „Error“ kontakt 2</t>
   </si>
 </sst>
 </file>
@@ -1704,7 +1782,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3416,7 +3494,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3585,10 +3663,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>193</v>
+        <v>212</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>128</v>
@@ -3599,10 +3677,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>195</v>
+        <v>214</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>128</v>
@@ -3627,7 +3705,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="H31" activeCellId="0" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3656,13 +3734,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3670,13 +3748,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3793,8 +3871,8 @@
   </sheetPr>
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3823,10 +3901,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>154</v>
@@ -3837,10 +3915,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>154</v>
@@ -3851,10 +3929,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>154</v>
@@ -3865,17 +3943,815 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>154</v>
       </c>
     </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0"/>
+      <c r="C14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0"/>
+      <c r="C15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0"/>
+      <c r="C16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0"/>
+      <c r="C17" s="0"/>
+    </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="5"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.72"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0"/>
+      <c r="C14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0"/>
+      <c r="C15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0"/>
+      <c r="C16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0"/>
+      <c r="C17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="5"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.72"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0"/>
+      <c r="C10" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0"/>
+      <c r="C14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0"/>
+      <c r="C15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0"/>
+      <c r="C16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0"/>
+      <c r="C17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="5"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F36" activeCellId="0" sqref="F36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.72"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0"/>
+      <c r="C10" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0"/>
+      <c r="C14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0"/>
+      <c r="C15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0"/>
+      <c r="C16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0"/>
+      <c r="C17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="5"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.79"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.72"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0"/>
+      <c r="C13" s="0"/>
+      <c r="D13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0"/>
+      <c r="C14" s="0"/>
+      <c r="D14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0"/>
+      <c r="C15" s="0"/>
+      <c r="D15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0"/>
+      <c r="C16" s="0"/>
+      <c r="D16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0"/>
+      <c r="C17" s="0"/>
+      <c r="D17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0"/>
+      <c r="C18" s="0"/>
+      <c r="D18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0"/>
+      <c r="C19" s="0"/>
+      <c r="D19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0"/>
+      <c r="C20" s="0"/>
+      <c r="D20" s="0"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0"/>
+      <c r="C21" s="0"/>
+      <c r="D21" s="0"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0"/>
+      <c r="C22" s="0"/>
+      <c r="D22" s="0"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0"/>
+      <c r="C23" s="0"/>
+      <c r="D23" s="0"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0"/>
+      <c r="C24" s="0"/>
+      <c r="D24" s="0"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0"/>
+      <c r="C25" s="0"/>
+      <c r="D25" s="0"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0"/>
+      <c r="C26" s="0"/>
+      <c r="D26" s="0"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
TGMmini dokonceno oprava oznaceni konektoru B2CF (bylo spatne BLZ)
</commit_message>
<xml_diff>
--- a/docs/Manual/source/CZ/tab/connectors.xlsx
+++ b/docs/Manual/source/CZ/tab/connectors.xlsx
@@ -5,18 +5,18 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="35"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="38"/>
   </bookViews>
   <sheets>
     <sheet name="rozcestnik" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="X1_24V_5pin_BCZ" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="X2_48_DC_1778065" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="X8_IO_22pin_BCZ" sheetId="4" state="visible" r:id="rId6"/>
-    <sheet name="X10_CAN_4pin_BCZ" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="X8_IO_22pin_B2CF" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="X10_CAN_4pin_B2CF" sheetId="5" state="visible" r:id="rId7"/>
     <sheet name="LEDsigAx12" sheetId="6" state="visible" r:id="rId8"/>
-    <sheet name="X5_FBE_12pin_BCZ" sheetId="7" state="visible" r:id="rId9"/>
-    <sheet name="X6_FB1_8pin_BCZ" sheetId="8" state="visible" r:id="rId10"/>
-    <sheet name="X7_FB2_8pin_BCZ" sheetId="9" state="visible" r:id="rId11"/>
+    <sheet name="X5_FBE_12pin_B2CF" sheetId="7" state="visible" r:id="rId9"/>
+    <sheet name="X6_FB1_8pin_B2CF" sheetId="8" state="visible" r:id="rId10"/>
+    <sheet name="X7_FB2_8pin_B2CF" sheetId="9" state="visible" r:id="rId11"/>
     <sheet name="X3_M1_6pin_BLZP" sheetId="10" state="visible" r:id="rId12"/>
     <sheet name="X4_M2_6pin_BLZP" sheetId="11" state="visible" r:id="rId13"/>
     <sheet name="X1_24V_5pin_Microlock" sheetId="12" state="visible" r:id="rId14"/>
@@ -44,6 +44,10 @@
     <sheet name="X1_ACIN_PC5" sheetId="34" state="visible" r:id="rId36"/>
     <sheet name="X2_DC_8pin_PC5" sheetId="35" state="visible" r:id="rId37"/>
     <sheet name="X3_DO_4pin_BCZ" sheetId="36" state="visible" r:id="rId38"/>
+    <sheet name="X3_24V_BLF_2_5" sheetId="37" state="visible" r:id="rId39"/>
+    <sheet name="X5_DI_10pin_B2CF" sheetId="38" state="visible" r:id="rId40"/>
+    <sheet name="X10_DO_10pin_B2CF" sheetId="39" state="visible" r:id="rId41"/>
+    <sheet name="S1_SWITCH_CAN" sheetId="40" state="visible" r:id="rId42"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -55,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="280">
   <si>
     <t xml:space="preserve">Toto je sešit se zdrojovými tabulkami popisu konektorů TGZ/TGS v češtině. Každý list odpovídá jednomu unikátnímu typu konektoru. Jelikož se často konektory v rámci TGZ opakují (typicky ty na řídicií desce), jsou zde jen jednou. Tj. Např. IO konektor 22pin weidmuller BCZ se používá pořád dokola, je zde tedy zanesen jen jednou jako „X8_IO_22pin_BCZ“</t>
   </si>
@@ -820,6 +824,117 @@
   </si>
   <si>
     <t xml:space="preserve">Signál „Error“ kontakt 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+PWR 24V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vstup pro napájecí napětí 24V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,08 ~ 0,5 mm2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PWRCOM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vstup pro napájecí zem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digitální vstup č. 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digitální vstup č. 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUT3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUT4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUT5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUT6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUT7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUT8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUTCOM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Společná zem DO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUTPWR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Společné napájení DO 24V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pozice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Funkce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nahoře</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vypnuto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAN není terminován</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zapnuto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAN je terminován</t>
   </si>
 </sst>
 </file>
@@ -3952,22 +4067,6 @@
         <v>154</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0"/>
-      <c r="C14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0"/>
-      <c r="C15" s="0"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0"/>
-      <c r="C16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0"/>
-      <c r="C17" s="0"/>
-    </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="5"/>
     </row>
@@ -4070,22 +4169,6 @@
         <v>154</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0"/>
-      <c r="C14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0"/>
-      <c r="C15" s="0"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0"/>
-      <c r="C16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0"/>
-      <c r="C17" s="0"/>
-    </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="5"/>
     </row>
@@ -4108,7 +4191,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4187,26 +4270,6 @@
       <c r="D5" s="1" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0"/>
-      <c r="C10" s="0"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0"/>
-      <c r="C14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0"/>
-      <c r="C15" s="0"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0"/>
-      <c r="C16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0"/>
-      <c r="C17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="5"/>
@@ -4310,26 +4373,6 @@
         <v>222</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0"/>
-      <c r="C10" s="0"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0"/>
-      <c r="C14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0"/>
-      <c r="C15" s="0"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0"/>
-      <c r="C16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0"/>
-      <c r="C17" s="0"/>
-    </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="5"/>
     </row>
@@ -4357,7 +4400,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4403,13 +4446,13 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>226</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -4432,7 +4475,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
@@ -4446,128 +4489,128 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>198</v>
       </c>
     </row>
@@ -4582,76 +4625,6 @@
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0"/>
-      <c r="C13" s="0"/>
-      <c r="D13" s="0"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0"/>
-      <c r="C14" s="0"/>
-      <c r="D14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0"/>
-      <c r="C15" s="0"/>
-      <c r="D15" s="0"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0"/>
-      <c r="C16" s="0"/>
-      <c r="D16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0"/>
-      <c r="C17" s="0"/>
-      <c r="D17" s="0"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0"/>
-      <c r="C18" s="0"/>
-      <c r="D18" s="0"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0"/>
-      <c r="C19" s="0"/>
-      <c r="D19" s="0"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0"/>
-      <c r="C20" s="0"/>
-      <c r="D20" s="0"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0"/>
-      <c r="C21" s="0"/>
-      <c r="D21" s="0"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0"/>
-      <c r="C22" s="0"/>
-      <c r="D22" s="0"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0"/>
-      <c r="C23" s="0"/>
-      <c r="D23" s="0"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0"/>
-      <c r="C24" s="0"/>
-      <c r="D24" s="0"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0"/>
-      <c r="C25" s="0"/>
-      <c r="D25" s="0"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0"/>
-      <c r="C26" s="0"/>
-      <c r="D26" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4671,8 +4644,8 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4752,6 +4725,424 @@
       <c r="D5" s="1" t="s">
         <v>34</v>
       </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="5"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5102,6 +5493,101 @@
       <c r="D23" s="1" t="s">
         <v>50</v>
       </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
dokoncen profinet pridan S-48-50RI - rozpracovano
</commit_message>
<xml_diff>
--- a/docs/Manual/source/CZ/tab/connectors.xlsx
+++ b/docs/Manual/source/CZ/tab/connectors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="49"/>
   </bookViews>
   <sheets>
     <sheet name="rozcestnik" sheetId="1" state="visible" r:id="rId3"/>
@@ -52,6 +52,12 @@
     <sheet name="X5_FBE_12pin_B2CF_TGM" sheetId="42" state="visible" r:id="rId44"/>
     <sheet name="X6_FB1_8pin_B2CF_TGM" sheetId="43" state="visible" r:id="rId45"/>
     <sheet name="X7_FB2_8pin_B2CF_TGM" sheetId="44" state="visible" r:id="rId46"/>
+    <sheet name="X4_FBE_12pin_ClikMate" sheetId="45" state="visible" r:id="rId47"/>
+    <sheet name="X5_FB1_10pin_ClikMate" sheetId="46" state="visible" r:id="rId48"/>
+    <sheet name="X6_FB2_10pin_ClikMate" sheetId="47" state="visible" r:id="rId49"/>
+    <sheet name="X7_AIN_12pin_ClikMate" sheetId="48" state="visible" r:id="rId50"/>
+    <sheet name="X8_DIO_18pin_ClikMate" sheetId="49" state="visible" r:id="rId51"/>
+    <sheet name="X10_CAN_8pin_ClikMate" sheetId="50" state="visible" r:id="rId52"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -63,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1573" uniqueCount="375">
   <si>
     <t xml:space="preserve">Toto je sešit se zdrojovými tabulkami popisu konektorů TGZ/TGS v češtině. Každý list odpovídá jednomu unikátnímu typu konektoru. Jelikož se často konektory v rámci TGZ opakují (typicky ty na řídicií desce), jsou zde jen jednou. Tj. Např. IO konektor 22pin weidmuller B2CF se používá pořád dokola, je zde tedy zanesen jen jednou jako „X8_IO_22pin_B2CF“</t>
   </si>
@@ -1081,6 +1087,150 @@
   <si>
     <t xml:space="preserve">SSI</t>
   </si>
+  <si>
+    <t xml:space="preserve">RS422, RS485</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MA+ (CLK+)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxD+/RxD+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MA- (CLK-)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TxD-/RxD-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SLO+ (DATA+)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SLO- (DATA-)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RxD+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RxD-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analogový vstup 0-10V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analogová zem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PT1000_1+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vstup pro 1. PT1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PT1000_1-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PT1000_2+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vstup pro 2. PT1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PT1000_2-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DITTL1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dig. Vstup 5-30V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digitální zem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DITTL2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DITTL3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digitální vstup izolovaný č. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digitální vstup izolovaný č. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digitální vstup izolovaný č. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digitální vstup izolovaný č. 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digitální vstup izolovaný č. 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digitální vstup izolovaný č. 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digitální vstup izolovaný č. 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digitální vstup izolovaný č. 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNDIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oddělená zem DO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VDDIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oddělené napájení DO 24V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digitální výstup izolovaný č. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digitální výstup izolovaný č. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digitální výstup izolovaný č. 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digitální výstup izolovaný č. 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digitální výstup izolovaný č. 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digitální výstup izolovaný č. 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAN High signál</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAN Low signál</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAN izolovaná zem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CANTH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAN terminační propoj H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CANTL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAN terminační propoj L</t>
+  </si>
 </sst>
 </file>
 
@@ -1090,7 +1240,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1113,13 +1263,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <charset val="238"/>
     </font>
     <font>
@@ -1191,7 +1334,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1204,11 +1347,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1224,19 +1363,7 @@
       <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1433,8 +1560,8 @@
   </sheetPr>
   <dimension ref="A1:H138"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B128" activeCellId="0" sqref="B128"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1545,16 +1672,16 @@
       <c r="D9" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E9" s="5" t="n">
+      <c r="E9" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="F9" s="5" t="n">
+      <c r="F9" s="4" t="n">
         <v>100</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1568,12 +1695,12 @@
       <c r="D10" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
       <c r="G10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1587,12 +1714,12 @@
       <c r="D11" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
       <c r="G11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1606,12 +1733,12 @@
       <c r="D12" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
       <c r="G12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="5" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1625,12 +1752,12 @@
       <c r="D13" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
       <c r="G13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1644,12 +1771,12 @@
       <c r="D14" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
       <c r="G14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1663,12 +1790,12 @@
       <c r="D15" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
       <c r="G15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1682,12 +1809,12 @@
       <c r="D16" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
       <c r="G16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1701,16 +1828,16 @@
       <c r="D17" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E17" s="5" t="n">
+      <c r="E17" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="F17" s="5" t="n">
+      <c r="F17" s="4" t="n">
         <v>250</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1724,12 +1851,12 @@
       <c r="D18" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
       <c r="G18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H18" s="7" t="s">
+      <c r="H18" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1743,12 +1870,12 @@
       <c r="D19" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
       <c r="G19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1762,12 +1889,12 @@
       <c r="D20" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
       <c r="G20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="5" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1781,12 +1908,12 @@
       <c r="D21" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
       <c r="G21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H21" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1800,12 +1927,12 @@
       <c r="D22" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
       <c r="G22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H22" s="6" t="s">
+      <c r="H22" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1819,8 +1946,8 @@
       <c r="D23" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
       <c r="G23" s="1" t="s">
         <v>24</v>
       </c>
@@ -1838,8 +1965,8 @@
       <c r="D24" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
       <c r="G24" s="1" t="s">
         <v>26</v>
       </c>
@@ -1857,16 +1984,16 @@
       <c r="D25" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E25" s="5" t="n">
+      <c r="E25" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="F25" s="5" t="n">
+      <c r="F25" s="4" t="n">
         <v>300</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="6" t="s">
+      <c r="H25" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1880,12 +2007,12 @@
       <c r="D26" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
       <c r="G26" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H26" s="7" t="s">
+      <c r="H26" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1899,12 +2026,12 @@
       <c r="D27" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
       <c r="G27" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="H27" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1918,12 +2045,12 @@
       <c r="D28" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
       <c r="G28" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="H28" s="5" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1937,12 +2064,12 @@
       <c r="D29" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
       <c r="G29" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H29" s="6" t="s">
+      <c r="H29" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1956,12 +2083,12 @@
       <c r="D30" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
       <c r="G30" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H30" s="6" t="s">
+      <c r="H30" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1975,8 +2102,8 @@
       <c r="D31" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
       <c r="G31" s="1" t="s">
         <v>24</v>
       </c>
@@ -1994,8 +2121,8 @@
       <c r="D32" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
       <c r="G32" s="1" t="s">
         <v>26</v>
       </c>
@@ -2013,16 +2140,16 @@
       <c r="D33" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E33" s="5" t="n">
+      <c r="E33" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="F33" s="5" t="n">
+      <c r="F33" s="4" t="n">
         <v>450</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H33" s="6" t="s">
+      <c r="H33" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2036,12 +2163,12 @@
       <c r="D34" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
       <c r="G34" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H34" s="7" t="s">
+      <c r="H34" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2055,12 +2182,12 @@
       <c r="D35" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
       <c r="G35" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H35" s="6" t="s">
+      <c r="H35" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2074,12 +2201,12 @@
       <c r="D36" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
       <c r="G36" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H36" s="6" t="s">
+      <c r="H36" s="5" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2093,12 +2220,12 @@
       <c r="D37" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
       <c r="G37" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H37" s="6" t="s">
+      <c r="H37" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2112,12 +2239,12 @@
       <c r="D38" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
       <c r="G38" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H38" s="6" t="s">
+      <c r="H38" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2131,8 +2258,8 @@
       <c r="D39" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
       <c r="G39" s="1" t="s">
         <v>24</v>
       </c>
@@ -2150,8 +2277,8 @@
       <c r="D40" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
       <c r="G40" s="1" t="s">
         <v>26</v>
       </c>
@@ -2169,16 +2296,16 @@
       <c r="D41" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E41" s="5" t="n">
+      <c r="E41" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="F41" s="5" t="n">
+      <c r="F41" s="4" t="n">
         <v>26</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H41" s="6" t="s">
+      <c r="H41" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2192,12 +2319,12 @@
       <c r="D42" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
       <c r="G42" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H42" s="7" t="s">
+      <c r="H42" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2211,12 +2338,12 @@
       <c r="D43" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
       <c r="G43" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H43" s="6" t="s">
+      <c r="H43" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2230,12 +2357,12 @@
       <c r="D44" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
       <c r="G44" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H44" s="6" t="s">
+      <c r="H44" s="5" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2249,12 +2376,12 @@
       <c r="D45" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
       <c r="G45" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H45" s="6" t="s">
+      <c r="H45" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2268,12 +2395,12 @@
       <c r="D46" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
       <c r="G46" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H46" s="6" t="s">
+      <c r="H46" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2287,12 +2414,12 @@
       <c r="D47" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
       <c r="G47" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H47" s="6" t="s">
+      <c r="H47" s="5" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2306,12 +2433,12 @@
       <c r="D48" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
       <c r="G48" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H48" s="6" t="s">
+      <c r="H48" s="5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2325,12 +2452,12 @@
       <c r="D49" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
       <c r="G49" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H49" s="6" t="s">
+      <c r="H49" s="5" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2344,16 +2471,16 @@
       <c r="D50" s="3" t="n">
         <v>230</v>
       </c>
-      <c r="E50" s="5" t="n">
+      <c r="E50" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="F50" s="5" t="n">
+      <c r="F50" s="4" t="n">
         <v>15</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H50" s="6" t="s">
+      <c r="H50" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2367,12 +2494,12 @@
       <c r="D51" s="3" t="n">
         <v>230</v>
       </c>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
       <c r="G51" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H51" s="7" t="s">
+      <c r="H51" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2386,12 +2513,12 @@
       <c r="D52" s="3" t="n">
         <v>230</v>
       </c>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
       <c r="G52" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H52" s="6" t="s">
+      <c r="H52" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2405,12 +2532,12 @@
       <c r="D53" s="3" t="n">
         <v>230</v>
       </c>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
       <c r="G53" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H53" s="6" t="s">
+      <c r="H53" s="5" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2424,12 +2551,12 @@
       <c r="D54" s="3" t="n">
         <v>230</v>
       </c>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
       <c r="G54" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H54" s="6" t="s">
+      <c r="H54" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2443,12 +2570,12 @@
       <c r="D55" s="3" t="n">
         <v>230</v>
       </c>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
       <c r="G55" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H55" s="6" t="s">
+      <c r="H55" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2462,12 +2589,12 @@
       <c r="D56" s="3" t="n">
         <v>230</v>
       </c>
-      <c r="E56" s="5"/>
-      <c r="F56" s="5"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
       <c r="G56" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H56" s="6" t="s">
+      <c r="H56" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2481,12 +2608,12 @@
       <c r="D57" s="3" t="n">
         <v>230</v>
       </c>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
       <c r="G57" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H57" s="6" t="s">
+      <c r="H57" s="5" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2500,16 +2627,16 @@
       <c r="D58" s="3" t="n">
         <v>320</v>
       </c>
-      <c r="E58" s="5" t="n">
+      <c r="E58" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="F58" s="5" t="n">
+      <c r="F58" s="4" t="n">
         <v>10</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H58" s="6" t="s">
+      <c r="H58" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2521,12 +2648,12 @@
         <v>29</v>
       </c>
       <c r="D59" s="3"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="5"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
       <c r="G59" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H59" s="7" t="s">
+      <c r="H59" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2538,12 +2665,12 @@
         <v>29</v>
       </c>
       <c r="D60" s="3"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
       <c r="G60" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H60" s="6" t="s">
+      <c r="H60" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2555,12 +2682,12 @@
         <v>29</v>
       </c>
       <c r="D61" s="3"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
       <c r="G61" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H61" s="6" t="s">
+      <c r="H61" s="5" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2572,12 +2699,12 @@
         <v>29</v>
       </c>
       <c r="D62" s="3"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="5"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
       <c r="G62" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H62" s="6" t="s">
+      <c r="H62" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2589,12 +2716,12 @@
         <v>29</v>
       </c>
       <c r="D63" s="3"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
       <c r="G63" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H63" s="6" t="s">
+      <c r="H63" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2606,12 +2733,12 @@
         <v>29</v>
       </c>
       <c r="D64" s="3"/>
-      <c r="E64" s="5"/>
-      <c r="F64" s="5"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
       <c r="G64" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H64" s="6" t="s">
+      <c r="H64" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2623,12 +2750,12 @@
         <v>29</v>
       </c>
       <c r="D65" s="3"/>
-      <c r="E65" s="5"/>
-      <c r="F65" s="5"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
       <c r="G65" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H65" s="6" t="s">
+      <c r="H65" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2640,12 +2767,12 @@
         <v>29</v>
       </c>
       <c r="D66" s="3"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="5"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
       <c r="G66" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H66" s="6" t="s">
+      <c r="H66" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2659,16 +2786,16 @@
       <c r="D67" s="3" t="n">
         <v>320</v>
       </c>
-      <c r="E67" s="5" t="n">
+      <c r="E67" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="F67" s="5" t="n">
+      <c r="F67" s="4" t="n">
         <v>15</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H67" s="6" t="s">
+      <c r="H67" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2680,12 +2807,12 @@
         <v>29</v>
       </c>
       <c r="D68" s="3"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="5"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
       <c r="G68" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H68" s="7" t="s">
+      <c r="H68" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2697,12 +2824,12 @@
         <v>29</v>
       </c>
       <c r="D69" s="3"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
+      <c r="E69" s="4"/>
+      <c r="F69" s="4"/>
       <c r="G69" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H69" s="6" t="s">
+      <c r="H69" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2714,12 +2841,12 @@
         <v>29</v>
       </c>
       <c r="D70" s="3"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="5"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
       <c r="G70" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H70" s="6" t="s">
+      <c r="H70" s="5" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2731,12 +2858,12 @@
         <v>29</v>
       </c>
       <c r="D71" s="3"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="5"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
       <c r="G71" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H71" s="6" t="s">
+      <c r="H71" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2748,12 +2875,12 @@
         <v>29</v>
       </c>
       <c r="D72" s="3"/>
-      <c r="E72" s="5"/>
-      <c r="F72" s="5"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="4"/>
       <c r="G72" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H72" s="6" t="s">
+      <c r="H72" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2765,12 +2892,12 @@
         <v>29</v>
       </c>
       <c r="D73" s="3"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="5"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
       <c r="G73" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H73" s="6" t="s">
+      <c r="H73" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2782,12 +2909,12 @@
         <v>29</v>
       </c>
       <c r="D74" s="3"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="5"/>
+      <c r="E74" s="4"/>
+      <c r="F74" s="4"/>
       <c r="G74" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H74" s="6" t="s">
+      <c r="H74" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2799,12 +2926,12 @@
         <v>29</v>
       </c>
       <c r="D75" s="3"/>
-      <c r="E75" s="5"/>
-      <c r="F75" s="5"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="4"/>
       <c r="G75" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H75" s="6" t="s">
+      <c r="H75" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2818,16 +2945,16 @@
       <c r="D76" s="3" t="n">
         <v>400</v>
       </c>
-      <c r="E76" s="8" t="n">
+      <c r="E76" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="F76" s="5" t="n">
+      <c r="F76" s="4" t="n">
         <v>9</v>
       </c>
       <c r="G76" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H76" s="6" t="s">
+      <c r="H76" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2839,12 +2966,12 @@
         <v>11</v>
       </c>
       <c r="D77" s="3"/>
-      <c r="E77" s="8"/>
-      <c r="F77" s="5"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
       <c r="G77" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H77" s="7" t="s">
+      <c r="H77" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2856,12 +2983,12 @@
         <v>11</v>
       </c>
       <c r="D78" s="3"/>
-      <c r="E78" s="8"/>
-      <c r="F78" s="5"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="4"/>
       <c r="G78" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H78" s="6" t="s">
+      <c r="H78" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2873,12 +3000,12 @@
         <v>11</v>
       </c>
       <c r="D79" s="3"/>
-      <c r="E79" s="8"/>
-      <c r="F79" s="5"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
       <c r="G79" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H79" s="6" t="s">
+      <c r="H79" s="5" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2890,12 +3017,12 @@
         <v>11</v>
       </c>
       <c r="D80" s="3"/>
-      <c r="E80" s="8"/>
-      <c r="F80" s="5"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="4"/>
       <c r="G80" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H80" s="6" t="s">
+      <c r="H80" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2907,12 +3034,12 @@
         <v>11</v>
       </c>
       <c r="D81" s="3"/>
-      <c r="E81" s="8"/>
-      <c r="F81" s="5"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="4"/>
       <c r="G81" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H81" s="6" t="s">
+      <c r="H81" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2924,12 +3051,12 @@
         <v>11</v>
       </c>
       <c r="D82" s="3"/>
-      <c r="E82" s="8"/>
-      <c r="F82" s="5"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="4"/>
       <c r="G82" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H82" s="6" t="s">
+      <c r="H82" s="5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2941,12 +3068,12 @@
         <v>11</v>
       </c>
       <c r="D83" s="3"/>
-      <c r="E83" s="8"/>
-      <c r="F83" s="5"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="4"/>
       <c r="G83" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H83" s="6" t="s">
+      <c r="H83" s="5" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2958,16 +3085,16 @@
         <v>11</v>
       </c>
       <c r="D84" s="3"/>
-      <c r="E84" s="8" t="n">
+      <c r="E84" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="F84" s="5" t="n">
+      <c r="F84" s="4" t="n">
         <v>15</v>
       </c>
       <c r="G84" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H84" s="6" t="s">
+      <c r="H84" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2979,12 +3106,12 @@
         <v>11</v>
       </c>
       <c r="D85" s="3"/>
-      <c r="E85" s="8"/>
-      <c r="F85" s="5"/>
+      <c r="E85" s="4"/>
+      <c r="F85" s="4"/>
       <c r="G85" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H85" s="7" t="s">
+      <c r="H85" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2996,12 +3123,12 @@
         <v>11</v>
       </c>
       <c r="D86" s="3"/>
-      <c r="E86" s="8"/>
-      <c r="F86" s="5"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="4"/>
       <c r="G86" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H86" s="6" t="s">
+      <c r="H86" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3013,12 +3140,12 @@
         <v>11</v>
       </c>
       <c r="D87" s="3"/>
-      <c r="E87" s="8"/>
-      <c r="F87" s="5"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="4"/>
       <c r="G87" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H87" s="6" t="s">
+      <c r="H87" s="5" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3030,12 +3157,12 @@
         <v>11</v>
       </c>
       <c r="D88" s="3"/>
-      <c r="E88" s="8"/>
-      <c r="F88" s="5"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="4"/>
       <c r="G88" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H88" s="6" t="s">
+      <c r="H88" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -3047,12 +3174,12 @@
         <v>11</v>
       </c>
       <c r="D89" s="3"/>
-      <c r="E89" s="8"/>
-      <c r="F89" s="5"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="4"/>
       <c r="G89" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H89" s="6" t="s">
+      <c r="H89" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3064,12 +3191,12 @@
         <v>11</v>
       </c>
       <c r="D90" s="3"/>
-      <c r="E90" s="8"/>
-      <c r="F90" s="5"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="4"/>
       <c r="G90" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H90" s="6" t="s">
+      <c r="H90" s="5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3081,12 +3208,12 @@
         <v>11</v>
       </c>
       <c r="D91" s="3"/>
-      <c r="E91" s="8"/>
-      <c r="F91" s="5"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="4"/>
       <c r="G91" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H91" s="6" t="s">
+      <c r="H91" s="5" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3098,16 +3225,16 @@
         <v>11</v>
       </c>
       <c r="D92" s="3"/>
-      <c r="E92" s="8" t="n">
-        <v>10</v>
-      </c>
-      <c r="F92" s="5" t="n">
+      <c r="E92" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="F92" s="4" t="n">
         <v>20</v>
       </c>
       <c r="G92" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H92" s="6" t="s">
+      <c r="H92" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3119,12 +3246,12 @@
         <v>11</v>
       </c>
       <c r="D93" s="3"/>
-      <c r="E93" s="8"/>
-      <c r="F93" s="5"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="4"/>
       <c r="G93" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H93" s="7" t="s">
+      <c r="H93" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3136,12 +3263,12 @@
         <v>11</v>
       </c>
       <c r="D94" s="3"/>
-      <c r="E94" s="8"/>
-      <c r="F94" s="5"/>
+      <c r="E94" s="4"/>
+      <c r="F94" s="4"/>
       <c r="G94" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H94" s="6" t="s">
+      <c r="H94" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3153,12 +3280,12 @@
         <v>11</v>
       </c>
       <c r="D95" s="3"/>
-      <c r="E95" s="8"/>
-      <c r="F95" s="5"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="4"/>
       <c r="G95" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H95" s="6" t="s">
+      <c r="H95" s="5" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3170,12 +3297,12 @@
         <v>11</v>
       </c>
       <c r="D96" s="3"/>
-      <c r="E96" s="8"/>
-      <c r="F96" s="5"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="4"/>
       <c r="G96" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H96" s="6" t="s">
+      <c r="H96" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -3187,12 +3314,12 @@
         <v>11</v>
       </c>
       <c r="D97" s="3"/>
-      <c r="E97" s="8"/>
-      <c r="F97" s="5"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="4"/>
       <c r="G97" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H97" s="6" t="s">
+      <c r="H97" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3204,12 +3331,12 @@
         <v>11</v>
       </c>
       <c r="D98" s="3"/>
-      <c r="E98" s="8"/>
-      <c r="F98" s="5"/>
+      <c r="E98" s="4"/>
+      <c r="F98" s="4"/>
       <c r="G98" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H98" s="6" t="s">
+      <c r="H98" s="5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3221,12 +3348,12 @@
         <v>11</v>
       </c>
       <c r="D99" s="3"/>
-      <c r="E99" s="8"/>
-      <c r="F99" s="5"/>
+      <c r="E99" s="4"/>
+      <c r="F99" s="4"/>
       <c r="G99" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H99" s="6" t="s">
+      <c r="H99" s="5" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3238,16 +3365,16 @@
         <v>11</v>
       </c>
       <c r="D100" s="3"/>
-      <c r="E100" s="8" t="n">
+      <c r="E100" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="F100" s="5" t="n">
+      <c r="F100" s="4" t="n">
         <v>30</v>
       </c>
       <c r="G100" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H100" s="6" t="s">
+      <c r="H100" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3259,12 +3386,12 @@
         <v>11</v>
       </c>
       <c r="D101" s="3"/>
-      <c r="E101" s="8"/>
-      <c r="F101" s="5"/>
+      <c r="E101" s="4"/>
+      <c r="F101" s="4"/>
       <c r="G101" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H101" s="7" t="s">
+      <c r="H101" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3276,12 +3403,12 @@
         <v>11</v>
       </c>
       <c r="D102" s="3"/>
-      <c r="E102" s="8"/>
-      <c r="F102" s="5"/>
+      <c r="E102" s="4"/>
+      <c r="F102" s="4"/>
       <c r="G102" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H102" s="6" t="s">
+      <c r="H102" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3293,12 +3420,12 @@
         <v>11</v>
       </c>
       <c r="D103" s="3"/>
-      <c r="E103" s="8"/>
-      <c r="F103" s="5"/>
+      <c r="E103" s="4"/>
+      <c r="F103" s="4"/>
       <c r="G103" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H103" s="6" t="s">
+      <c r="H103" s="5" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3310,12 +3437,12 @@
         <v>11</v>
       </c>
       <c r="D104" s="3"/>
-      <c r="E104" s="8"/>
-      <c r="F104" s="5"/>
+      <c r="E104" s="4"/>
+      <c r="F104" s="4"/>
       <c r="G104" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H104" s="6" t="s">
+      <c r="H104" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -3327,12 +3454,12 @@
         <v>11</v>
       </c>
       <c r="D105" s="3"/>
-      <c r="E105" s="8"/>
-      <c r="F105" s="5"/>
+      <c r="E105" s="4"/>
+      <c r="F105" s="4"/>
       <c r="G105" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H105" s="6" t="s">
+      <c r="H105" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3344,12 +3471,12 @@
         <v>11</v>
       </c>
       <c r="D106" s="3"/>
-      <c r="E106" s="8"/>
-      <c r="F106" s="5"/>
+      <c r="E106" s="4"/>
+      <c r="F106" s="4"/>
       <c r="G106" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H106" s="6" t="s">
+      <c r="H106" s="5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3361,12 +3488,12 @@
         <v>11</v>
       </c>
       <c r="D107" s="3"/>
-      <c r="E107" s="8"/>
-      <c r="F107" s="5"/>
+      <c r="E107" s="4"/>
+      <c r="F107" s="4"/>
       <c r="G107" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H107" s="6" t="s">
+      <c r="H107" s="5" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3377,19 +3504,19 @@
       <c r="C108" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D108" s="8" t="n">
+      <c r="D108" s="4" t="n">
         <v>560</v>
       </c>
-      <c r="E108" s="5" t="n">
+      <c r="E108" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="F108" s="5" t="n">
+      <c r="F108" s="4" t="n">
         <v>50</v>
       </c>
       <c r="G108" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H108" s="6" t="s">
+      <c r="H108" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3398,13 +3525,13 @@
         <v>10</v>
       </c>
       <c r="C109" s="3"/>
-      <c r="D109" s="8"/>
-      <c r="E109" s="5"/>
-      <c r="F109" s="5"/>
+      <c r="D109" s="4"/>
+      <c r="E109" s="4"/>
+      <c r="F109" s="4"/>
       <c r="G109" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H109" s="7" t="s">
+      <c r="H109" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3413,13 +3540,13 @@
         <v>10</v>
       </c>
       <c r="C110" s="3"/>
-      <c r="D110" s="8"/>
-      <c r="E110" s="5"/>
-      <c r="F110" s="5"/>
+      <c r="D110" s="4"/>
+      <c r="E110" s="4"/>
+      <c r="F110" s="4"/>
       <c r="G110" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H110" s="6" t="s">
+      <c r="H110" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3428,13 +3555,13 @@
         <v>10</v>
       </c>
       <c r="C111" s="3"/>
-      <c r="D111" s="8"/>
-      <c r="E111" s="5"/>
-      <c r="F111" s="5"/>
+      <c r="D111" s="4"/>
+      <c r="E111" s="4"/>
+      <c r="F111" s="4"/>
       <c r="G111" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H111" s="6" t="s">
+      <c r="H111" s="5" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3443,13 +3570,13 @@
         <v>10</v>
       </c>
       <c r="C112" s="3"/>
-      <c r="D112" s="8"/>
-      <c r="E112" s="5"/>
-      <c r="F112" s="5"/>
+      <c r="D112" s="4"/>
+      <c r="E112" s="4"/>
+      <c r="F112" s="4"/>
       <c r="G112" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H112" s="6" t="s">
+      <c r="H112" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -3458,13 +3585,13 @@
         <v>10</v>
       </c>
       <c r="C113" s="3"/>
-      <c r="D113" s="8"/>
-      <c r="E113" s="5"/>
-      <c r="F113" s="5"/>
+      <c r="D113" s="4"/>
+      <c r="E113" s="4"/>
+      <c r="F113" s="4"/>
       <c r="G113" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H113" s="6" t="s">
+      <c r="H113" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3473,13 +3600,13 @@
         <v>10</v>
       </c>
       <c r="C114" s="3"/>
-      <c r="D114" s="8"/>
-      <c r="E114" s="5"/>
-      <c r="F114" s="5"/>
+      <c r="D114" s="4"/>
+      <c r="E114" s="4"/>
+      <c r="F114" s="4"/>
       <c r="G114" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H114" s="6" t="s">
+      <c r="H114" s="5" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3488,13 +3615,13 @@
         <v>10</v>
       </c>
       <c r="C115" s="3"/>
-      <c r="D115" s="8"/>
-      <c r="E115" s="5"/>
-      <c r="F115" s="5"/>
+      <c r="D115" s="4"/>
+      <c r="E115" s="4"/>
+      <c r="F115" s="4"/>
       <c r="G115" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H115" s="6" t="s">
+      <c r="H115" s="5" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3503,13 +3630,13 @@
         <v>10</v>
       </c>
       <c r="C116" s="3"/>
-      <c r="D116" s="8"/>
-      <c r="E116" s="5"/>
-      <c r="F116" s="5"/>
+      <c r="D116" s="4"/>
+      <c r="E116" s="4"/>
+      <c r="F116" s="4"/>
       <c r="G116" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H116" s="6" t="s">
+      <c r="H116" s="5" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3520,11 +3647,11 @@
       <c r="C117" s="3"/>
       <c r="D117" s="3"/>
       <c r="E117" s="3"/>
-      <c r="F117" s="5"/>
+      <c r="F117" s="4"/>
       <c r="G117" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H117" s="9" t="s">
+      <c r="H117" s="5" t="s">
         <v>46</v>
       </c>
     </row>
@@ -3535,25 +3662,25 @@
       <c r="C118" s="3"/>
       <c r="D118" s="3"/>
       <c r="E118" s="3"/>
-      <c r="F118" s="5"/>
+      <c r="F118" s="4"/>
       <c r="G118" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H118" s="9" t="s">
+      <c r="H118" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B119" s="10" t="s">
+      <c r="B119" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C119" s="10" t="s">
+      <c r="C119" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D119" s="8" t="n">
+      <c r="D119" s="4" t="n">
         <v>320</v>
       </c>
-      <c r="E119" s="8" t="n">
+      <c r="E119" s="4" t="n">
         <v>10</v>
       </c>
       <c r="F119" s="4" t="n">
@@ -3562,55 +3689,55 @@
       <c r="G119" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H119" s="9" t="s">
+      <c r="H119" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B120" s="10" t="s">
+      <c r="B120" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C120" s="10" t="s">
+      <c r="C120" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D120" s="8"/>
-      <c r="E120" s="8"/>
+      <c r="D120" s="4"/>
+      <c r="E120" s="4"/>
       <c r="F120" s="4"/>
       <c r="G120" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H120" s="9" t="s">
+      <c r="H120" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B121" s="10" t="s">
+      <c r="B121" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C121" s="10" t="s">
+      <c r="C121" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D121" s="8"/>
-      <c r="E121" s="8"/>
+      <c r="D121" s="4"/>
+      <c r="E121" s="4"/>
       <c r="F121" s="4"/>
       <c r="G121" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H121" s="9" t="s">
+      <c r="H121" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B122" s="10" t="s">
+      <c r="B122" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C122" s="10" t="s">
+      <c r="C122" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D122" s="8" t="n">
+      <c r="D122" s="4" t="n">
         <v>560</v>
       </c>
-      <c r="E122" s="8" t="n">
+      <c r="E122" s="4" t="n">
         <v>25</v>
       </c>
       <c r="F122" s="4" t="n">
@@ -3621,44 +3748,44 @@
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B123" s="10" t="s">
+      <c r="B123" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C123" s="10" t="s">
+      <c r="C123" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D123" s="8"/>
-      <c r="E123" s="8"/>
+      <c r="D123" s="4"/>
+      <c r="E123" s="4"/>
       <c r="F123" s="4"/>
       <c r="G123" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B124" s="10" t="s">
+      <c r="B124" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C124" s="10" t="s">
+      <c r="C124" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D124" s="8"/>
-      <c r="E124" s="8"/>
+      <c r="D124" s="4"/>
+      <c r="E124" s="4"/>
       <c r="F124" s="4"/>
       <c r="G124" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B125" s="10" t="s">
+      <c r="B125" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C125" s="10" t="s">
+      <c r="C125" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D125" s="8" t="n">
+      <c r="D125" s="4" t="n">
         <v>560</v>
       </c>
-      <c r="E125" s="8" t="n">
+      <c r="E125" s="4" t="n">
         <v>50</v>
       </c>
       <c r="F125" s="4" t="n">
@@ -3669,179 +3796,179 @@
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B126" s="10" t="s">
+      <c r="B126" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C126" s="10" t="s">
+      <c r="C126" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D126" s="8"/>
-      <c r="E126" s="8"/>
+      <c r="D126" s="4"/>
+      <c r="E126" s="4"/>
       <c r="F126" s="4"/>
       <c r="G126" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B127" s="10" t="s">
+      <c r="B127" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C127" s="10" t="s">
+      <c r="C127" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D127" s="8"/>
-      <c r="E127" s="8"/>
+      <c r="D127" s="4"/>
+      <c r="E127" s="4"/>
       <c r="F127" s="4"/>
       <c r="G127" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B128" s="8" t="s">
+      <c r="B128" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C128" s="10" t="s">
+      <c r="C128" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D128" s="10"/>
-      <c r="E128" s="10"/>
-      <c r="F128" s="10"/>
+      <c r="D128" s="3"/>
+      <c r="E128" s="3"/>
+      <c r="F128" s="3"/>
       <c r="G128" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H128" s="9" t="s">
+      <c r="H128" s="5" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B129" s="8"/>
-      <c r="C129" s="10"/>
-      <c r="D129" s="10"/>
-      <c r="E129" s="10"/>
-      <c r="F129" s="10"/>
+      <c r="B129" s="4"/>
+      <c r="C129" s="3"/>
+      <c r="D129" s="3"/>
+      <c r="E129" s="3"/>
+      <c r="F129" s="3"/>
       <c r="G129" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H129" s="6" t="s">
+      <c r="H129" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B130" s="8"/>
-      <c r="C130" s="10"/>
-      <c r="D130" s="10"/>
-      <c r="E130" s="10"/>
-      <c r="F130" s="10"/>
-      <c r="G130" s="0" t="s">
+      <c r="B130" s="4"/>
+      <c r="C130" s="3"/>
+      <c r="D130" s="3"/>
+      <c r="E130" s="3"/>
+      <c r="F130" s="3"/>
+      <c r="G130" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H130" s="9" t="s">
+      <c r="H130" s="5" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B131" s="8"/>
-      <c r="C131" s="10"/>
-      <c r="D131" s="10"/>
-      <c r="E131" s="10"/>
-      <c r="F131" s="10"/>
+      <c r="B131" s="4"/>
+      <c r="C131" s="3"/>
+      <c r="D131" s="3"/>
+      <c r="E131" s="3"/>
+      <c r="F131" s="3"/>
       <c r="G131" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H131" s="9" t="s">
+      <c r="H131" s="5" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B132" s="8"/>
-      <c r="C132" s="10"/>
-      <c r="D132" s="10"/>
-      <c r="E132" s="10"/>
-      <c r="F132" s="10"/>
+      <c r="B132" s="4"/>
+      <c r="C132" s="3"/>
+      <c r="D132" s="3"/>
+      <c r="E132" s="3"/>
+      <c r="F132" s="3"/>
       <c r="G132" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H132" s="9" t="s">
+      <c r="H132" s="5" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B133" s="8"/>
-      <c r="C133" s="10" t="s">
+      <c r="B133" s="4"/>
+      <c r="C133" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D133" s="10"/>
-      <c r="E133" s="10"/>
-      <c r="F133" s="10"/>
+      <c r="D133" s="3"/>
+      <c r="E133" s="3"/>
+      <c r="F133" s="3"/>
       <c r="G133" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H133" s="9" t="s">
+      <c r="H133" s="5" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B134" s="8"/>
-      <c r="C134" s="8"/>
-      <c r="D134" s="10"/>
-      <c r="E134" s="10"/>
-      <c r="F134" s="10"/>
+      <c r="B134" s="4"/>
+      <c r="C134" s="4"/>
+      <c r="D134" s="3"/>
+      <c r="E134" s="3"/>
+      <c r="F134" s="3"/>
       <c r="G134" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H134" s="6" t="s">
+      <c r="H134" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B135" s="8"/>
-      <c r="C135" s="8"/>
-      <c r="D135" s="10"/>
-      <c r="E135" s="10"/>
-      <c r="F135" s="10"/>
+      <c r="B135" s="4"/>
+      <c r="C135" s="4"/>
+      <c r="D135" s="3"/>
+      <c r="E135" s="3"/>
+      <c r="F135" s="3"/>
       <c r="G135" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H135" s="7" t="s">
+      <c r="H135" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B136" s="8"/>
-      <c r="C136" s="8"/>
-      <c r="D136" s="10"/>
-      <c r="E136" s="10"/>
-      <c r="F136" s="10"/>
+      <c r="B136" s="4"/>
+      <c r="C136" s="4"/>
+      <c r="D136" s="3"/>
+      <c r="E136" s="3"/>
+      <c r="F136" s="3"/>
       <c r="G136" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H136" s="6" t="s">
+      <c r="H136" s="5" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B137" s="8"/>
-      <c r="C137" s="8"/>
-      <c r="D137" s="10"/>
-      <c r="E137" s="10"/>
-      <c r="F137" s="10"/>
+      <c r="B137" s="4"/>
+      <c r="C137" s="4"/>
+      <c r="D137" s="3"/>
+      <c r="E137" s="3"/>
+      <c r="F137" s="3"/>
       <c r="G137" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H137" s="6" t="s">
+      <c r="H137" s="5" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B138" s="8"/>
-      <c r="C138" s="8"/>
-      <c r="D138" s="10"/>
-      <c r="E138" s="10"/>
-      <c r="F138" s="10"/>
+      <c r="B138" s="4"/>
+      <c r="C138" s="4"/>
+      <c r="D138" s="3"/>
+      <c r="E138" s="3"/>
+      <c r="F138" s="3"/>
       <c r="G138" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H138" s="6" t="s">
+      <c r="H138" s="5" t="s">
         <v>68</v>
       </c>
     </row>
@@ -4144,7 +4271,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="11"/>
+      <c r="C18" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4274,7 +4401,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="11"/>
+      <c r="C18" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4461,7 +4588,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="11"/>
+      <c r="C18" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4549,7 +4676,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="11"/>
+      <c r="C18" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4736,7 +4863,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="11"/>
+      <c r="C18" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4838,7 +4965,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="11"/>
+      <c r="C18" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4940,7 +5067,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="11"/>
+      <c r="C18" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4989,7 +5116,7 @@
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="8" t="s">
         <v>197</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -5046,7 +5173,7 @@
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="8" t="s">
         <v>203</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -5060,7 +5187,7 @@
       <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="8" t="s">
         <v>205</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -5071,7 +5198,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="11"/>
+      <c r="C18" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5700,7 +5827,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="11"/>
+      <c r="C18" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5732,161 +5859,161 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="9" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="n">
+      <c r="A2" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="9" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="n">
+      <c r="A3" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="9" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="n">
+      <c r="A4" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="9" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="n">
+      <c r="A5" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="9" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13" t="n">
+      <c r="A6" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="9" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="n">
+      <c r="A7" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="9" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="n">
+      <c r="A8" s="9" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="9" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="n">
+      <c r="A9" s="9" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="9" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13" t="n">
+      <c r="A10" s="9" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="9" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" s="13" t="s">
+      <c r="A11" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="9" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="11"/>
+      <c r="C18" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -6099,7 +6226,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="11"/>
+      <c r="C18" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -6579,7 +6706,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="11"/>
+      <c r="C18" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -6681,7 +6808,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="11"/>
+      <c r="C18" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -6783,7 +6910,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="11"/>
+      <c r="C18" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -6885,7 +7012,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="11"/>
+      <c r="C18" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -7126,16 +7253,16 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -7494,7 +7621,7 @@
       <c r="A13" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="11"/>
+      <c r="C18" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -7653,7 +7780,7 @@
       <c r="A13" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="11"/>
+      <c r="C18" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -7674,7 +7801,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8098,7 +8225,7 @@
       <c r="A13" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="11"/>
+      <c r="C18" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -8474,7 +8601,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="11"/>
+      <c r="C18" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -8605,7 +8732,1216 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="11"/>
+      <c r="B18" s="7"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E29"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.99"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>332</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="7"/>
+      <c r="D18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D20" s="0"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D21" s="0"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D22" s="0"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D23" s="0"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D24" s="0"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D25" s="0"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D27" s="0"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D28" s="0"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D29" s="0"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E27"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.99"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>332</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="7"/>
+      <c r="D16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D20" s="0"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D21" s="0"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D22" s="0"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D23" s="0"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D24" s="0"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D25" s="0"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D27" s="0"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E27"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.99"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>332</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="7"/>
+      <c r="D16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D20" s="0"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D21" s="0"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D22" s="0"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D23" s="0"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D24" s="0"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D25" s="0"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D27" s="0"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="7"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>367</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -8703,6 +10039,134 @@
       </c>
       <c r="D5" s="1" t="s">
         <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -8968,7 +10432,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="11"/>
+      <c r="C18" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -8989,7 +10453,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9126,7 +10590,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="11"/>
+      <c r="C18" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -9284,7 +10748,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="11"/>
+      <c r="C18" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
odstraneny chyby pri kompilaci (cesty k souboru upper/lower case) upravy dle Petronela, fakticke chyby v man
</commit_message>
<xml_diff>
--- a/docs/Manual/source/CZ/tab/connectors.xlsx
+++ b/docs/Manual/source/CZ/tab/connectors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="52"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="rozcestnik" sheetId="1" state="visible" r:id="rId3"/>
@@ -791,7 +791,7 @@
     <t xml:space="preserve">0,75 ~ 16 mm2</t>
   </si>
   <si>
-    <t xml:space="preserve">0,2 ~ 10 mm2</t>
+    <t xml:space="preserve">0,2 ~ 6 mm2</t>
   </si>
   <si>
     <t xml:space="preserve">-B2</t>
@@ -1765,8 +1765,8 @@
   </sheetPr>
   <dimension ref="A1:K138"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I29" activeCellId="0" sqref="I29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6825,8 +6825,8 @@
   </sheetPr>
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6928,7 +6928,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12357,7 +12357,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
@@ -12367,147 +12367,107 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="49.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0"/>
-      <c r="C10" s="0"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0"/>
-      <c r="C11" s="0"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0"/>
-      <c r="C12" s="0"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0"/>
-      <c r="C13" s="0"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0"/>
-      <c r="C14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0"/>
-      <c r="C15" s="0"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0"/>
-      <c r="C16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0"/>
-      <c r="C17" s="0"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0"/>
-      <c r="C18" s="0"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0"/>
-      <c r="C19" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -12535,7 +12495,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12556,7 +12516,7 @@
       <c r="B2" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>410</v>
       </c>
     </row>
@@ -12567,7 +12527,7 @@
       <c r="B3" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>412</v>
       </c>
     </row>
@@ -12578,7 +12538,7 @@
       <c r="B4" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>413</v>
       </c>
     </row>
@@ -12589,7 +12549,7 @@
       <c r="B5" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>414</v>
       </c>
     </row>
@@ -12600,7 +12560,7 @@
       <c r="B6" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>416</v>
       </c>
     </row>
@@ -12611,7 +12571,7 @@
       <c r="B7" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>417</v>
       </c>
     </row>
@@ -12622,7 +12582,7 @@
       <c r="B8" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>418</v>
       </c>
     </row>
@@ -12633,7 +12593,7 @@
       <c r="B9" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>419</v>
       </c>
     </row>
@@ -12644,7 +12604,7 @@
       <c r="B10" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>420</v>
       </c>
     </row>
@@ -12655,7 +12615,7 @@
       <c r="B11" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>421</v>
       </c>
     </row>
@@ -12686,7 +12646,7 @@
   </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -12694,115 +12654,113 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="29.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>427</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>431</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>433</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>435</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
-      <c r="C10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1"/>
-      <c r="C11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>

</xml_diff>